<commit_message>
Updated Relatório & Mockups
</commit_message>
<xml_diff>
--- a/gantt.xlsx
+++ b/gantt.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="33600" windowHeight="21000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="projeto" sheetId="1" r:id="rId1"/>
@@ -524,17 +524,17 @@
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Activity" xfId="2"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Cabeçalho 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Hiperligação" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Label" xfId="5"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percent Complete" xfId="6"/>
@@ -708,7 +708,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="periodo_selecionado" max="60" min="1" page="10"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="periodo_selecionado" max="60" min="1" page="10" val="4"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -718,19 +718,19 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>19</xdr:col>
-          <xdr:colOff>63500</xdr:colOff>
+          <xdr:colOff>66675</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>19</xdr:col>
-          <xdr:colOff>203200</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>60960</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1029" name="Controle Giratório 5" hidden="1">
+            <xdr:cNvPr id="1029" name="Controle Giratório 5" descr="Period Highlight Spin Control" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1029"/>
@@ -739,7 +739,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -747,6 +747,12 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData fPrintsWithSheet="0"/>
@@ -1017,7 +1023,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Ion" id="{B8441ADB-2E43-4AF7-B97A-BD870242C6A8}" vid="{292E63A9-BB86-4E3D-B92A-7223C6510D2E}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Ion" id="{B8441ADB-2E43-4AF7-B97A-BD870242C6A8}" vid="{292E63A9-BB86-4E3D-B92A-7223C6510D2E}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1025,27 +1031,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B2:AA27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.85546875" defaultRowHeight="17" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" style="2" customWidth="1"/>
-    <col min="3" max="5" width="7.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="4.28515625" style="1" customWidth="1"/>
-    <col min="9" max="26" width="2.85546875" style="1"/>
+    <col min="1" max="1" width="3.875" customWidth="1"/>
+    <col min="2" max="2" width="53.375" style="2" customWidth="1"/>
+    <col min="3" max="5" width="7.25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.375" style="7" customWidth="1"/>
+    <col min="8" max="8" width="4.25" style="1" customWidth="1"/>
+    <col min="9" max="26" width="2.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:27" ht="15" customHeight="1">
+    <row r="2" spans="2:27" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="23" t="s">
         <v>12</v>
       </c>
@@ -1067,11 +1073,11 @@
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
       <c r="S2" s="19">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="T2" s="8"/>
     </row>
-    <row r="3" spans="2:27" ht="21" customHeight="1">
+    <row r="3" spans="2:27" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
@@ -1082,7 +1088,7 @@
       <c r="I3" s="23"/>
       <c r="J3" s="23"/>
     </row>
-    <row r="4" spans="2:27" ht="18.75" customHeight="1">
+    <row r="4" spans="2:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="23"/>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
@@ -1108,7 +1114,7 @@
       <c r="W4"/>
       <c r="X4"/>
     </row>
-    <row r="5" spans="2:27">
+    <row r="5" spans="2:27" x14ac:dyDescent="0.3">
       <c r="O5"/>
       <c r="P5"/>
       <c r="Q5"/>
@@ -1122,7 +1128,7 @@
       <c r="Y5"/>
       <c r="Z5"/>
     </row>
-    <row r="6" spans="2:27" ht="15">
+    <row r="6" spans="2:27" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
         <v>1</v>
@@ -1157,7 +1163,7 @@
       <c r="V6"/>
       <c r="W6"/>
     </row>
-    <row r="7" spans="2:27" ht="13.5" customHeight="1">
+    <row r="7" spans="2:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
@@ -1194,7 +1200,7 @@
       <c r="Y7"/>
       <c r="Z7"/>
     </row>
-    <row r="8" spans="2:27" ht="15.75" customHeight="1">
+    <row r="8" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1258,7 +1264,7 @@
       </c>
       <c r="AA8" s="1"/>
     </row>
-    <row r="9" spans="2:27" ht="19" customHeight="1">
+    <row r="9" spans="2:27" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
@@ -1278,7 +1284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:27" ht="18.75" customHeight="1">
+    <row r="10" spans="2:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="21" t="s">
         <v>13</v>
       </c>
@@ -1298,7 +1304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:27" ht="19" customHeight="1">
+    <row r="11" spans="2:27" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="21" t="s">
         <v>14</v>
       </c>
@@ -1318,7 +1324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:27" ht="19" customHeight="1">
+    <row r="12" spans="2:27" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="21" t="s">
         <v>15</v>
       </c>
@@ -1338,7 +1344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:27" ht="19" customHeight="1">
+    <row r="13" spans="2:27" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="21" t="s">
         <v>16</v>
       </c>
@@ -1358,7 +1364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:27" ht="19" customHeight="1">
+    <row r="14" spans="2:27" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="20" t="s">
         <v>18</v>
       </c>
@@ -1378,7 +1384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:27" ht="19" customHeight="1">
+    <row r="15" spans="2:27" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="21" t="s">
         <v>19</v>
       </c>
@@ -1398,7 +1404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:27" ht="19" customHeight="1">
+    <row r="16" spans="2:27" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="21" t="s">
         <v>20</v>
       </c>
@@ -1418,7 +1424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="19" customHeight="1">
+    <row r="17" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="21" t="s">
         <v>21</v>
       </c>
@@ -1438,7 +1444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="19" customHeight="1">
+    <row r="18" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="21" t="s">
         <v>22</v>
       </c>
@@ -1458,7 +1464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="19" customHeight="1">
+    <row r="19" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="21" t="s">
         <v>23</v>
       </c>
@@ -1478,7 +1484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="19" customHeight="1">
+    <row r="20" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="21" t="s">
         <v>24</v>
       </c>
@@ -1498,7 +1504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="19" customHeight="1">
+    <row r="21" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="21" t="s">
         <v>25</v>
       </c>
@@ -1518,7 +1524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="19" customHeight="1">
+    <row r="22" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="20" t="s">
         <v>26</v>
       </c>
@@ -1538,7 +1544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="19" customHeight="1">
+    <row r="23" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="21" t="s">
         <v>27</v>
       </c>
@@ -1558,7 +1564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="19" customHeight="1">
+    <row r="24" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="21" t="s">
         <v>28</v>
       </c>
@@ -1578,7 +1584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="19" customHeight="1">
+    <row r="25" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="21" t="s">
         <v>29</v>
       </c>
@@ -1598,7 +1604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="19" customHeight="1">
+    <row r="26" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
@@ -1606,7 +1612,7 @@
       <c r="F26" s="15"/>
       <c r="G26" s="16"/>
     </row>
-    <row r="27" spans="2:7" ht="19" customHeight="1">
+    <row r="27" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
@@ -1668,25 +1674,23 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>19</xdr:col>
-                    <xdr:colOff>63500</xdr:colOff>
+                    <xdr:colOff>66675</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>25400</xdr:rowOff>
+                    <xdr:rowOff>28575</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>19</xdr:col>
-                    <xdr:colOff>203200</xdr:colOff>
+                    <xdr:colOff>200025</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>63500</xdr:rowOff>
+                    <xdr:rowOff>66675</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
       </controls>
     </mc:Choice>
-    <mc:Fallback/>
   </mc:AlternateContent>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>